<commit_message>
Update PCB as per manufacturing requirements
</commit_message>
<xml_diff>
--- a/pcb_design/BoM.xlsx
+++ b/pcb_design/BoM.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="330">
   <si>
     <t>MUSHAK BILL OF MATERIALS</t>
   </si>
@@ -226,7 +226,7 @@
     <t>C11, C15,</t>
   </si>
   <si>
-    <t>20pF (22uF * avaiable)</t>
+    <t>22pF</t>
   </si>
   <si>
     <t>0402N220J500CT</t>
@@ -495,7 +495,7 @@
     <t>RC0402FR-0710KL</t>
   </si>
   <si>
-    <t>Resistor &gt;</t>
+    <t xml:space="preserve">Resistor </t>
   </si>
   <si>
     <t>R7, R12, R23, R24,</t>
@@ -507,9 +507,6 @@
     <t>0603SAJ0101T5E</t>
   </si>
   <si>
-    <t xml:space="preserve">d'. </t>
-  </si>
-  <si>
     <t>R27, R28, R29, R30, R31</t>
   </si>
   <si>
@@ -519,9 +516,6 @@
     <t>0402WGF1500TCE</t>
   </si>
   <si>
-    <t>d';l f[</t>
-  </si>
-  <si>
     <t>SW1, SW2,</t>
   </si>
   <si>
@@ -555,7 +549,7 @@
     <t>U3,</t>
   </si>
   <si>
-    <t>DRV8833PWPR</t>
+    <t>DRV8833PW</t>
   </si>
   <si>
     <t>Package_SO:TSSOP-16_4.4x5mm_P0.65mm</t>
@@ -961,9 +955,6 @@
   </si>
   <si>
     <t xml:space="preserve">U3, </t>
-  </si>
-  <si>
-    <t>DRV8833PW</t>
   </si>
   <si>
     <t>DRV8833 (₹99)</t>
@@ -2000,7 +1991,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="39.0"/>
+    <col customWidth="1" min="1" max="1" width="51.0"/>
     <col customWidth="1" min="2" max="2" width="8.0"/>
     <col customWidth="1" min="3" max="3" width="17.63"/>
     <col customWidth="1" min="4" max="5" width="28.75"/>
@@ -3585,7 +3576,7 @@
         <v>134</v>
       </c>
       <c r="F28" s="51" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G28" s="56"/>
       <c r="H28" s="56"/>
@@ -3629,22 +3620,22 @@
     </row>
     <row r="29">
       <c r="A29" s="51" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B29" s="51">
         <v>5.0</v>
       </c>
       <c r="C29" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="51" t="s">
         <v>157</v>
-      </c>
-      <c r="D29" s="51" t="s">
-        <v>158</v>
       </c>
       <c r="E29" s="51" t="s">
         <v>146</v>
       </c>
       <c r="F29" s="51" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="G29" s="56"/>
       <c r="H29" s="56"/>
@@ -3682,22 +3673,22 @@
     </row>
     <row r="30">
       <c r="A30" s="52" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B30" s="52">
         <v>2.0</v>
       </c>
       <c r="C30" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="D30" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="E30" s="52" t="s">
         <v>161</v>
       </c>
-      <c r="D30" s="51" t="s">
+      <c r="F30" s="52" t="s">
         <v>162</v>
-      </c>
-      <c r="E30" s="52" t="s">
-        <v>163</v>
-      </c>
-      <c r="F30" s="52" t="s">
-        <v>164</v>
       </c>
       <c r="G30" s="56"/>
       <c r="H30" s="56"/>
@@ -3742,27 +3733,27 @@
     </row>
     <row r="31">
       <c r="A31" s="51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B31" s="52">
         <v>1.0</v>
       </c>
       <c r="C31" s="51" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" s="51" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="F31" s="51" t="s">
         <v>166</v>
-      </c>
-      <c r="D31" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="E31" s="51" t="s">
-        <v>167</v>
-      </c>
-      <c r="F31" s="51" t="s">
-        <v>168</v>
       </c>
       <c r="G31" s="82"/>
       <c r="H31" s="82"/>
       <c r="I31" s="34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J31" s="51">
         <v>100.78</v>
@@ -3801,22 +3792,22 @@
     </row>
     <row r="32">
       <c r="A32" s="83" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B32" s="83">
         <v>1.0</v>
       </c>
       <c r="C32" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="E32" s="83" t="s">
+        <v>170</v>
+      </c>
+      <c r="F32" s="83" t="s">
         <v>171</v>
-      </c>
-      <c r="D32" s="84" t="s">
-        <v>171</v>
-      </c>
-      <c r="E32" s="83" t="s">
-        <v>172</v>
-      </c>
-      <c r="F32" s="83" t="s">
-        <v>173</v>
       </c>
       <c r="G32" s="85" t="s">
         <v>38</v>
@@ -3827,18 +3818,18 @@
       <c r="I32" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="J32" s="73">
-        <v>209.34</v>
+      <c r="J32" s="74">
+        <v>242.0</v>
       </c>
       <c r="K32" s="76">
         <f t="shared" si="7"/>
-        <v>209.34</v>
+        <v>242</v>
       </c>
       <c r="L32" s="78">
         <v>1.0</v>
       </c>
       <c r="M32" s="78">
-        <v>209.34</v>
+        <v>242.34</v>
       </c>
       <c r="N32" s="76"/>
       <c r="O32" s="79">
@@ -3846,7 +3837,7 @@
         <v>3.4858</v>
       </c>
       <c r="P32" s="75" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Q32" s="74">
         <v>3.4858</v>
@@ -3854,22 +3845,22 @@
     </row>
     <row r="33">
       <c r="A33" s="52" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B33" s="52">
         <v>1.0</v>
       </c>
       <c r="C33" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="E33" s="52" t="s">
+        <v>175</v>
+      </c>
+      <c r="F33" s="51" t="s">
         <v>176</v>
-      </c>
-      <c r="D33" s="51" t="s">
-        <v>176</v>
-      </c>
-      <c r="E33" s="52" t="s">
-        <v>177</v>
-      </c>
-      <c r="F33" s="51" t="s">
-        <v>178</v>
       </c>
       <c r="G33" s="75" t="s">
         <v>38</v>
@@ -3878,7 +3869,7 @@
         <v>39</v>
       </c>
       <c r="I33" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J33" s="74">
         <v>648.0</v>
@@ -3899,7 +3890,7 @@
         <v>3.2063</v>
       </c>
       <c r="P33" s="75" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q33" s="74">
         <v>3.2063</v>
@@ -3907,22 +3898,22 @@
     </row>
     <row r="34">
       <c r="A34" s="83" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B34" s="83">
         <v>1.0</v>
       </c>
       <c r="C34" s="83" t="s">
+        <v>180</v>
+      </c>
+      <c r="D34" s="83" t="s">
+        <v>180</v>
+      </c>
+      <c r="E34" s="83" t="s">
+        <v>181</v>
+      </c>
+      <c r="F34" s="84" t="s">
         <v>182</v>
-      </c>
-      <c r="D34" s="83" t="s">
-        <v>182</v>
-      </c>
-      <c r="E34" s="83" t="s">
-        <v>183</v>
-      </c>
-      <c r="F34" s="84" t="s">
-        <v>184</v>
       </c>
       <c r="G34" s="85" t="s">
         <v>38</v>
@@ -3931,7 +3922,7 @@
         <v>39</v>
       </c>
       <c r="I34" s="88" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J34" s="73">
         <v>727.89</v>
@@ -3952,7 +3943,7 @@
         <v>3.5651</v>
       </c>
       <c r="P34" s="75" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="Q34" s="74">
         <v>3.5651</v>
@@ -3960,22 +3951,22 @@
     </row>
     <row r="35">
       <c r="A35" s="73" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B35" s="73">
         <v>1.0</v>
       </c>
       <c r="C35" s="74" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" s="74" t="s">
+        <v>186</v>
+      </c>
+      <c r="E35" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="F35" s="73" t="s">
         <v>188</v>
-      </c>
-      <c r="D35" s="74" t="s">
-        <v>188</v>
-      </c>
-      <c r="E35" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="F35" s="73" t="s">
-        <v>190</v>
       </c>
       <c r="G35" s="87" t="s">
         <v>38</v>
@@ -4002,7 +3993,7 @@
         <v>10.1327</v>
       </c>
       <c r="P35" s="75" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="Q35" s="74">
         <v>10.1327</v>
@@ -4010,27 +4001,27 @@
     </row>
     <row r="36">
       <c r="A36" s="52" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B36" s="52">
         <v>1.0</v>
       </c>
       <c r="C36" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="D36" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="E36" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="D36" s="51" t="s">
+      <c r="F36" s="52" t="s">
         <v>194</v>
-      </c>
-      <c r="E36" s="52" t="s">
-        <v>195</v>
-      </c>
-      <c r="F36" s="52" t="s">
-        <v>196</v>
       </c>
       <c r="G36" s="56"/>
       <c r="H36" s="56"/>
       <c r="I36" s="64" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J36" s="51">
         <v>34.69</v>
@@ -4052,7 +4043,7 @@
         <v>0.8782</v>
       </c>
       <c r="P36" s="63" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Q36" s="51">
         <v>0.8782</v>
@@ -4072,25 +4063,25 @@
     </row>
     <row r="37">
       <c r="A37" s="52" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B37" s="52">
         <v>1.0</v>
       </c>
       <c r="C37" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="D37" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="E37" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="D37" s="51" t="s">
+      <c r="F37" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="E37" s="52" t="s">
+      <c r="G37" s="91" t="s">
         <v>202</v>
-      </c>
-      <c r="F37" s="52" t="s">
-        <v>203</v>
-      </c>
-      <c r="G37" s="91" t="s">
-        <v>204</v>
       </c>
       <c r="H37" s="56"/>
       <c r="I37" s="64" t="s">
@@ -4116,7 +4107,7 @@
         <v>0.1737</v>
       </c>
       <c r="P37" s="63" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q37" s="51">
         <v>0.1737</v>
@@ -4136,7 +4127,7 @@
     </row>
     <row r="38">
       <c r="A38" s="92" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B38" s="93">
         <f>SUM(B2:B37)</f>
@@ -4145,11 +4136,11 @@
     </row>
     <row r="39">
       <c r="L39" s="94" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M39" s="95">
         <f>SUM(M6:M37)</f>
-        <v>5648.85</v>
+        <v>5681.85</v>
       </c>
       <c r="N39" s="76"/>
     </row>
@@ -4432,7 +4423,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="92" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H1" s="99"/>
       <c r="I1" s="99"/>
@@ -4580,7 +4571,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="107" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E6" s="51" t="s">
         <v>10</v>
@@ -4601,7 +4592,7 @@
         <v>21</v>
       </c>
       <c r="K6" s="110" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L6" s="111" t="s">
         <v>17</v>
@@ -4610,7 +4601,7 @@
         <v>16</v>
       </c>
       <c r="N6" s="113" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="O6" s="114" t="s">
         <v>19</v>
@@ -4618,7 +4609,7 @@
     </row>
     <row r="7">
       <c r="A7" s="115" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B7" s="115">
         <v>4.0</v>
@@ -4633,7 +4624,7 @@
         <v>26</v>
       </c>
       <c r="F7" s="115" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G7" s="116" t="s">
         <v>30</v>
@@ -4661,12 +4652,12 @@
         <v>498.58</v>
       </c>
       <c r="O7" s="92" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="115" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B8" s="115">
         <v>1.0</v>
@@ -4715,7 +4706,7 @@
     </row>
     <row r="9">
       <c r="A9" s="115" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B9" s="115">
         <v>3.0</v>
@@ -4724,7 +4715,7 @@
         <v>44</v>
       </c>
       <c r="D9" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E9" s="115" t="s">
         <v>56</v>
@@ -4742,7 +4733,7 @@
         <v>49</v>
       </c>
       <c r="J9" s="121" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K9" s="119">
         <v>2.12</v>
@@ -4763,7 +4754,7 @@
     </row>
     <row r="10">
       <c r="A10" s="115" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B10" s="115">
         <v>5.0</v>
@@ -4772,7 +4763,7 @@
         <v>54</v>
       </c>
       <c r="D10" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E10" s="115" t="s">
         <v>56</v>
@@ -4805,21 +4796,21 @@
         <v>49.0</v>
       </c>
       <c r="O10" s="92" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="115" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B11" s="115">
         <v>2.0</v>
       </c>
       <c r="C11" s="115" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D11" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E11" s="115" t="s">
         <v>56</v>
@@ -4831,10 +4822,10 @@
         <v>50</v>
       </c>
       <c r="H11" s="122" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I11" s="122" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J11" s="116" t="s">
         <v>64</v>
@@ -4855,16 +4846,16 @@
     </row>
     <row r="12">
       <c r="A12" s="115" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B12" s="115">
         <v>2.0</v>
       </c>
       <c r="C12" s="115" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D12" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E12" s="115" t="s">
         <v>56</v>
@@ -4901,7 +4892,7 @@
     </row>
     <row r="13">
       <c r="A13" s="115" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B13" s="115">
         <v>2.0</v>
@@ -4910,7 +4901,7 @@
         <v>71</v>
       </c>
       <c r="D13" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E13" s="115" t="s">
         <v>56</v>
@@ -4942,16 +4933,16 @@
     </row>
     <row r="14">
       <c r="A14" s="115" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B14" s="115">
         <v>2.0</v>
       </c>
       <c r="C14" s="115" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D14" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E14" s="115" t="s">
         <v>56</v>
@@ -4983,7 +4974,7 @@
     </row>
     <row r="15">
       <c r="A15" s="115" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B15" s="115">
         <v>4.0</v>
@@ -4992,7 +4983,7 @@
         <v>79</v>
       </c>
       <c r="D15" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E15" s="115" t="s">
         <v>56</v>
@@ -5004,7 +4995,7 @@
         <v>50</v>
       </c>
       <c r="H15" s="117" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I15" s="123"/>
       <c r="J15" s="115"/>
@@ -5027,16 +5018,16 @@
     </row>
     <row r="16">
       <c r="A16" s="115" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B16" s="115">
         <v>7.0</v>
       </c>
       <c r="C16" s="115" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D16" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E16" s="115" t="s">
         <v>56</v>
@@ -5045,13 +5036,13 @@
         <v>47</v>
       </c>
       <c r="G16" s="121" t="s">
+        <v>232</v>
+      </c>
+      <c r="H16" s="125" t="s">
+        <v>233</v>
+      </c>
+      <c r="I16" s="117" t="s">
         <v>234</v>
-      </c>
-      <c r="H16" s="125" t="s">
-        <v>235</v>
-      </c>
-      <c r="I16" s="117" t="s">
-        <v>236</v>
       </c>
       <c r="J16" s="115"/>
       <c r="K16" s="119">
@@ -5071,16 +5062,16 @@
     </row>
     <row r="17">
       <c r="A17" s="115" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B17" s="115">
         <v>2.0</v>
       </c>
       <c r="C17" s="115" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D17" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E17" s="115" t="s">
         <v>56</v>
@@ -5089,13 +5080,13 @@
         <v>47</v>
       </c>
       <c r="G17" s="126" t="s">
+        <v>237</v>
+      </c>
+      <c r="H17" s="117" t="s">
+        <v>238</v>
+      </c>
+      <c r="I17" s="117" t="s">
         <v>239</v>
-      </c>
-      <c r="H17" s="117" t="s">
-        <v>240</v>
-      </c>
-      <c r="I17" s="117" t="s">
-        <v>241</v>
       </c>
       <c r="J17" s="115"/>
       <c r="K17" s="119">
@@ -5115,7 +5106,7 @@
     </row>
     <row r="18">
       <c r="A18" s="115" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B18" s="115">
         <v>1.0</v>
@@ -5124,7 +5115,7 @@
         <v>87</v>
       </c>
       <c r="D18" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E18" s="115" t="s">
         <v>56</v>
@@ -5133,13 +5124,13 @@
         <v>47</v>
       </c>
       <c r="G18" s="126" t="s">
+        <v>241</v>
+      </c>
+      <c r="H18" s="117" t="s">
+        <v>242</v>
+      </c>
+      <c r="I18" s="117" t="s">
         <v>243</v>
-      </c>
-      <c r="H18" s="117" t="s">
-        <v>244</v>
-      </c>
-      <c r="I18" s="117" t="s">
-        <v>245</v>
       </c>
       <c r="J18" s="115"/>
       <c r="K18" s="119">
@@ -5159,7 +5150,7 @@
     </row>
     <row r="19">
       <c r="A19" s="115" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B19" s="115">
         <v>1.0</v>
@@ -5168,7 +5159,7 @@
         <v>76</v>
       </c>
       <c r="D19" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E19" s="115" t="s">
         <v>56</v>
@@ -5177,13 +5168,13 @@
         <v>47</v>
       </c>
       <c r="G19" s="126" t="s">
+        <v>245</v>
+      </c>
+      <c r="H19" s="117" t="s">
+        <v>246</v>
+      </c>
+      <c r="I19" s="117" t="s">
         <v>247</v>
-      </c>
-      <c r="H19" s="117" t="s">
-        <v>248</v>
-      </c>
-      <c r="I19" s="117" t="s">
-        <v>249</v>
       </c>
       <c r="J19" s="115"/>
       <c r="K19" s="119">
@@ -5203,7 +5194,7 @@
     </row>
     <row r="20">
       <c r="A20" s="115" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B20" s="115">
         <v>2.0</v>
@@ -5237,7 +5228,7 @@
     </row>
     <row r="21">
       <c r="A21" s="115" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B21" s="115">
         <v>4.0</v>
@@ -5252,7 +5243,7 @@
         <v>99</v>
       </c>
       <c r="F21" s="115" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G21" s="128"/>
       <c r="H21" s="117" t="s">
@@ -5275,7 +5266,7 @@
     </row>
     <row r="22">
       <c r="A22" s="115" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B22" s="115">
         <v>1.0</v>
@@ -5284,7 +5275,7 @@
         <v>106</v>
       </c>
       <c r="D22" s="115" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E22" s="115" t="s">
         <v>108</v>
@@ -5309,29 +5300,29 @@
     </row>
     <row r="23">
       <c r="A23" s="115" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B23" s="115">
         <v>2.0</v>
       </c>
       <c r="C23" s="115" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D23" s="115" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E23" s="115" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F23" s="115" t="s">
         <v>114</v>
       </c>
       <c r="G23" s="128"/>
       <c r="H23" s="117" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I23" s="117" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J23" s="115"/>
       <c r="K23" s="123"/>
@@ -5347,7 +5338,7 @@
     </row>
     <row r="24">
       <c r="A24" s="115" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B24" s="115">
         <v>1.0</v>
@@ -5359,15 +5350,15 @@
         <v>117</v>
       </c>
       <c r="E24" s="115" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F24" s="115" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G24" s="127"/>
       <c r="H24" s="123"/>
       <c r="I24" s="119" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J24" s="115"/>
       <c r="K24" s="123"/>
@@ -5383,7 +5374,7 @@
     </row>
     <row r="25">
       <c r="A25" s="115" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B25" s="115">
         <v>1.0</v>
@@ -5398,7 +5389,7 @@
         <v>125</v>
       </c>
       <c r="F25" s="115" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G25" s="127"/>
       <c r="H25" s="123"/>
@@ -5417,7 +5408,7 @@
     </row>
     <row r="26">
       <c r="A26" s="115" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B26" s="115">
         <v>5.0</v>
@@ -5426,7 +5417,7 @@
         <v>128</v>
       </c>
       <c r="D26" s="115" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E26" s="115" t="s">
         <v>129</v>
@@ -5451,16 +5442,16 @@
     </row>
     <row r="27">
       <c r="A27" s="115" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B27" s="115">
         <v>1.0</v>
       </c>
       <c r="C27" s="115" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D27" s="115" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E27" s="115" t="s">
         <v>146</v>
@@ -5469,7 +5460,7 @@
         <v>135</v>
       </c>
       <c r="G27" s="121" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H27" s="117" t="s">
         <v>136</v>
@@ -5493,16 +5484,16 @@
     </row>
     <row r="28">
       <c r="A28" s="115" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B28" s="115">
         <v>2.0</v>
       </c>
       <c r="C28" s="115" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D28" s="115" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E28" s="115" t="s">
         <v>146</v>
@@ -5512,10 +5503,10 @@
       </c>
       <c r="G28" s="128"/>
       <c r="H28" s="117" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I28" s="117" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J28" s="115"/>
       <c r="K28" s="123"/>
@@ -5531,16 +5522,16 @@
     </row>
     <row r="29">
       <c r="A29" s="115" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B29" s="115">
         <v>2.0</v>
       </c>
       <c r="C29" s="115" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D29" s="115" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E29" s="115" t="s">
         <v>146</v>
@@ -5549,11 +5540,11 @@
         <v>135</v>
       </c>
       <c r="G29" s="121" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H29" s="123"/>
       <c r="I29" s="117" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J29" s="115"/>
       <c r="K29" s="119">
@@ -5573,7 +5564,7 @@
     </row>
     <row r="30">
       <c r="A30" s="115" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B30" s="115">
         <v>10.0</v>
@@ -5582,7 +5573,7 @@
         <v>144</v>
       </c>
       <c r="D30" s="115" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E30" s="115" t="s">
         <v>146</v>
@@ -5591,13 +5582,13 @@
         <v>135</v>
       </c>
       <c r="G30" s="121" t="s">
+        <v>279</v>
+      </c>
+      <c r="H30" s="117" t="s">
+        <v>280</v>
+      </c>
+      <c r="I30" s="117" t="s">
         <v>281</v>
-      </c>
-      <c r="H30" s="117" t="s">
-        <v>282</v>
-      </c>
-      <c r="I30" s="117" t="s">
-        <v>283</v>
       </c>
       <c r="J30" s="115"/>
       <c r="K30" s="119">
@@ -5617,16 +5608,16 @@
     </row>
     <row r="31">
       <c r="A31" s="115" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B31" s="115">
         <v>4.0</v>
       </c>
       <c r="C31" s="115" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D31" s="115" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E31" s="115" t="s">
         <v>146</v>
@@ -5635,13 +5626,13 @@
         <v>135</v>
       </c>
       <c r="G31" s="126" t="s">
+        <v>284</v>
+      </c>
+      <c r="H31" s="117" t="s">
+        <v>285</v>
+      </c>
+      <c r="I31" s="117" t="s">
         <v>286</v>
-      </c>
-      <c r="H31" s="117" t="s">
-        <v>287</v>
-      </c>
-      <c r="I31" s="117" t="s">
-        <v>288</v>
       </c>
       <c r="J31" s="115"/>
       <c r="K31" s="119">
@@ -5661,7 +5652,7 @@
     </row>
     <row r="32">
       <c r="A32" s="115" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B32" s="115">
         <v>5.0</v>
@@ -5670,7 +5661,7 @@
         <v>149</v>
       </c>
       <c r="D32" s="115" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E32" s="115" t="s">
         <v>146</v>
@@ -5679,10 +5670,10 @@
         <v>135</v>
       </c>
       <c r="G32" s="121" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H32" s="117" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I32" s="118" t="s">
         <v>32</v>
@@ -5705,16 +5696,16 @@
     </row>
     <row r="33">
       <c r="A33" s="115" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B33" s="115">
         <v>1.0</v>
       </c>
       <c r="C33" s="115" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D33" s="115" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E33" s="115" t="s">
         <v>146</v>
@@ -5723,13 +5714,13 @@
         <v>135</v>
       </c>
       <c r="G33" s="121" t="s">
+        <v>292</v>
+      </c>
+      <c r="H33" s="117" t="s">
+        <v>293</v>
+      </c>
+      <c r="I33" s="117" t="s">
         <v>294</v>
-      </c>
-      <c r="H33" s="117" t="s">
-        <v>295</v>
-      </c>
-      <c r="I33" s="117" t="s">
-        <v>296</v>
       </c>
       <c r="J33" s="115"/>
       <c r="K33" s="119">
@@ -5749,27 +5740,27 @@
     </row>
     <row r="34">
       <c r="A34" s="115" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B34" s="115">
         <v>2.0</v>
       </c>
       <c r="C34" s="115" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D34" s="115" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E34" s="115" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F34" s="115" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G34" s="127"/>
       <c r="H34" s="123"/>
       <c r="I34" s="117" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J34" s="115"/>
       <c r="K34" s="123"/>
@@ -5785,25 +5776,25 @@
     </row>
     <row r="35">
       <c r="A35" s="115" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B35" s="115">
         <v>1.0</v>
       </c>
       <c r="C35" s="115" t="s">
+        <v>299</v>
+      </c>
+      <c r="D35" s="115" t="s">
+        <v>300</v>
+      </c>
+      <c r="E35" s="115" t="s">
         <v>301</v>
       </c>
-      <c r="D35" s="115" t="s">
+      <c r="F35" s="115" t="s">
         <v>302</v>
       </c>
-      <c r="E35" s="115" t="s">
+      <c r="G35" s="121" t="s">
         <v>303</v>
-      </c>
-      <c r="F35" s="115" t="s">
-        <v>304</v>
-      </c>
-      <c r="G35" s="121" t="s">
-        <v>305</v>
       </c>
       <c r="H35" s="129"/>
       <c r="I35" s="129"/>
@@ -5823,25 +5814,25 @@
     </row>
     <row r="36">
       <c r="A36" s="115" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B36" s="115">
         <v>1.0</v>
       </c>
       <c r="C36" s="115" t="s">
-        <v>307</v>
+        <v>169</v>
       </c>
       <c r="D36" s="115" t="s">
-        <v>307</v>
+        <v>169</v>
       </c>
       <c r="E36" s="115" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F36" s="115" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G36" s="121" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H36" s="118" t="s">
         <v>32</v>
@@ -5865,31 +5856,31 @@
     </row>
     <row r="37">
       <c r="A37" s="115" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B37" s="115">
         <v>1.0</v>
       </c>
       <c r="C37" s="115" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D37" s="115" t="s">
+        <v>307</v>
+      </c>
+      <c r="E37" s="115" t="s">
+        <v>175</v>
+      </c>
+      <c r="F37" s="115" t="s">
+        <v>308</v>
+      </c>
+      <c r="G37" s="130" t="s">
+        <v>309</v>
+      </c>
+      <c r="H37" s="121" t="s">
         <v>310</v>
       </c>
-      <c r="E37" s="115" t="s">
-        <v>177</v>
-      </c>
-      <c r="F37" s="115" t="s">
+      <c r="I37" s="117" t="s">
         <v>311</v>
-      </c>
-      <c r="G37" s="130" t="s">
-        <v>312</v>
-      </c>
-      <c r="H37" s="121" t="s">
-        <v>313</v>
-      </c>
-      <c r="I37" s="117" t="s">
-        <v>314</v>
       </c>
       <c r="J37" s="123"/>
       <c r="K37" s="119">
@@ -5907,28 +5898,28 @@
     </row>
     <row r="38">
       <c r="A38" s="115" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B38" s="115">
         <v>1.0</v>
       </c>
       <c r="C38" s="115" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D38" s="115" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E38" s="115" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F38" s="115" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G38" s="121" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="H38" s="117" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="I38" s="118" t="s">
         <v>32</v>
@@ -5949,29 +5940,29 @@
     </row>
     <row r="39">
       <c r="A39" s="115" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B39" s="115">
         <v>1.0</v>
       </c>
       <c r="C39" s="115" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D39" s="115" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E39" s="115" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F39" s="115" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G39" s="128"/>
       <c r="H39" s="118" t="s">
         <v>32</v>
       </c>
       <c r="I39" s="117" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="J39" s="123"/>
       <c r="K39" s="123"/>
@@ -5987,31 +5978,31 @@
     </row>
     <row r="40">
       <c r="A40" s="115" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B40" s="115">
         <v>1.0</v>
       </c>
       <c r="C40" s="115" t="s">
+        <v>191</v>
+      </c>
+      <c r="D40" s="115" t="s">
+        <v>320</v>
+      </c>
+      <c r="E40" s="115" t="s">
         <v>193</v>
       </c>
-      <c r="D40" s="115" t="s">
+      <c r="F40" s="115" t="s">
+        <v>194</v>
+      </c>
+      <c r="G40" s="121" t="s">
+        <v>321</v>
+      </c>
+      <c r="H40" s="117" t="s">
+        <v>322</v>
+      </c>
+      <c r="I40" s="117" t="s">
         <v>323</v>
-      </c>
-      <c r="E40" s="115" t="s">
-        <v>195</v>
-      </c>
-      <c r="F40" s="115" t="s">
-        <v>196</v>
-      </c>
-      <c r="G40" s="121" t="s">
-        <v>324</v>
-      </c>
-      <c r="H40" s="117" t="s">
-        <v>325</v>
-      </c>
-      <c r="I40" s="117" t="s">
-        <v>326</v>
       </c>
       <c r="J40" s="123"/>
       <c r="K40" s="119">
@@ -6029,31 +6020,31 @@
     </row>
     <row r="41">
       <c r="A41" s="115" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B41" s="115">
         <v>1.0</v>
       </c>
       <c r="C41" s="115" t="s">
+        <v>325</v>
+      </c>
+      <c r="D41" s="115" t="s">
+        <v>326</v>
+      </c>
+      <c r="E41" s="115" t="s">
+        <v>200</v>
+      </c>
+      <c r="F41" s="115" t="s">
+        <v>201</v>
+      </c>
+      <c r="G41" s="121" t="s">
+        <v>327</v>
+      </c>
+      <c r="H41" s="117" t="s">
         <v>328</v>
       </c>
-      <c r="D41" s="115" t="s">
+      <c r="I41" s="117" t="s">
         <v>329</v>
-      </c>
-      <c r="E41" s="115" t="s">
-        <v>202</v>
-      </c>
-      <c r="F41" s="115" t="s">
-        <v>203</v>
-      </c>
-      <c r="G41" s="121" t="s">
-        <v>330</v>
-      </c>
-      <c r="H41" s="117" t="s">
-        <v>331</v>
-      </c>
-      <c r="I41" s="117" t="s">
-        <v>332</v>
       </c>
       <c r="J41" s="123"/>
       <c r="K41" s="119">

</xml_diff>

<commit_message>
Updated PCB with HTSSOP16 package for DRV8833
</commit_message>
<xml_diff>
--- a/pcb_design/BoM.xlsx
+++ b/pcb_design/BoM.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="332">
   <si>
     <t>MUSHAK BILL OF MATERIALS</t>
   </si>
@@ -549,412 +549,418 @@
     <t>U3,</t>
   </si>
   <si>
+    <t>DRV8833PWPR</t>
+  </si>
+  <si>
+    <t>Package_SO:HTSSOP-16_4.4x5mm_P0.65mm</t>
+  </si>
+  <si>
+    <t>Dual H-Bridge Motor Driver, TSSOP-16</t>
+  </si>
+  <si>
+    <t>C50506</t>
+  </si>
+  <si>
+    <t>U4,</t>
+  </si>
+  <si>
+    <t>VL6180XV0NR/1</t>
+  </si>
+  <si>
+    <t>VL6180XV0NR_1:LGA12R75P2X6_280X480X110</t>
+  </si>
+  <si>
+    <t>ToF</t>
+  </si>
+  <si>
+    <t>tanotis</t>
+  </si>
+  <si>
+    <t>C2688732</t>
+  </si>
+  <si>
+    <t>U5,</t>
+  </si>
+  <si>
+    <t>MPU-6500</t>
+  </si>
+  <si>
+    <t>MPU-6500:QFN40P300X300X95-25N</t>
+  </si>
+  <si>
+    <t>IMU</t>
+  </si>
+  <si>
+    <t>Not available in India (from module)</t>
+  </si>
+  <si>
+    <t>C50278</t>
+  </si>
+  <si>
+    <t>U6,</t>
+  </si>
+  <si>
+    <t>STM32F405RGT6</t>
+  </si>
+  <si>
+    <t>Package_QFP:LQFP-64_10x10mm_P0.5mm</t>
+  </si>
+  <si>
+    <t>ARM Cortex-M4 MCU, 1024KB flash, 128KB RAM, 168MHz, 1.8-3.6V, 51 GPIO, LQFP-64</t>
+  </si>
+  <si>
+    <t>C15742</t>
+  </si>
+  <si>
+    <t>Y1,</t>
+  </si>
+  <si>
+    <t>25Mhz</t>
+  </si>
+  <si>
+    <t>EC-9631</t>
+  </si>
+  <si>
+    <t>Crystal:Crystal_SMD_3225-4Pin_3.2x2.5mm</t>
+  </si>
+  <si>
+    <t>Four pin crystal, GND on pins 2 and 4</t>
+  </si>
+  <si>
+    <t>electronicscomp</t>
+  </si>
+  <si>
+    <t>C295525</t>
+  </si>
+  <si>
+    <t>Y2,</t>
+  </si>
+  <si>
+    <t>32.768kHz</t>
+  </si>
+  <si>
+    <t>X3215-32.768K-12.5</t>
+  </si>
+  <si>
+    <t>ABS07-32:XTAL_ABS07-32.768KHZ-T</t>
+  </si>
+  <si>
+    <t>Two pin crystal</t>
+  </si>
+  <si>
+    <t>assign footprint</t>
+  </si>
+  <si>
+    <t>C93228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of SMD components = </t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>di</t>
+  </si>
+  <si>
+    <t>Comp name</t>
+  </si>
+  <si>
+    <t>Best Buy (₹) /peice</t>
+  </si>
+  <si>
+    <t>Overall cost (₹)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1, A2, A3, A4, </t>
+  </si>
+  <si>
+    <t>Photo-Transistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available on Indian sites </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BZ1, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1, C2, C27, </t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C417153_$0.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3, C4, C30, C32, C33, </t>
+  </si>
+  <si>
+    <t>pack of 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8, C13, </t>
+  </si>
+  <si>
+    <t>47uF</t>
+  </si>
+  <si>
+    <t>47uf_0603 (₹30.84/10 piece)</t>
+  </si>
+  <si>
+    <t>47uF_0603 (₹36.97/10 piece)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C11, C15, </t>
+  </si>
+  <si>
+    <t>20pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C12, C19, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C20, C21, </t>
+  </si>
+  <si>
+    <t>12.5pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22, C24, C28, C18, </t>
+  </si>
+  <si>
+    <t>10uF_0402 (₹10.07/10 piece)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7, C9, C10, C14, C16, , C23, C25, </t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>100nF_0402 (₹1.78/40 piece)</t>
+  </si>
+  <si>
+    <t>too costly</t>
+  </si>
+  <si>
+    <t>100nF_0402 (₹2.86/10 piece)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C26, C17, </t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>10nF_0603 (₹2/50 piece)</t>
+  </si>
+  <si>
+    <t>10nF_0402 (₹8.79/10 piece)</t>
+  </si>
+  <si>
+    <t>10nF_0402 (₹13.28/10 piece)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C29, </t>
+  </si>
+  <si>
+    <t>4.7uF_0603 (₹1.8/10 piece)</t>
+  </si>
+  <si>
+    <t>4.7_0402 (₹21.97/10 piece)</t>
+  </si>
+  <si>
+    <t>4.7uF_0402 (₹19.16/10 piece)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C31, </t>
+  </si>
+  <si>
+    <t>0.01uF_0603 (₹1.8/10 piece)</t>
+  </si>
+  <si>
+    <t>(0.01uF (₹10.31/10 piece)</t>
+  </si>
+  <si>
+    <t>0.01uF (₹11.93/10 piece)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1, D6, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2, D3, D4, D5, </t>
+  </si>
+  <si>
+    <t>IR LED Transmitter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB1, </t>
+  </si>
+  <si>
+    <t>FerriteBead_Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC1, IC2, </t>
+  </si>
+  <si>
+    <t>AS5600-ASOT</t>
+  </si>
+  <si>
+    <t>AS5600-ASOT:SOIC127P600X175-8N</t>
+  </si>
+  <si>
+    <t>AS5600-ASOT (₹269.26)</t>
+  </si>
+  <si>
+    <t>AS5600-ASOT (₹267.92)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1, </t>
+  </si>
+  <si>
+    <t>Connector_JST:JST_SH_SM04B-SRSS-TB_1x04-1MP_P1.00mm_Horizontal</t>
+  </si>
+  <si>
+    <t>Serial Wire connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2, </t>
+  </si>
+  <si>
+    <t>Power connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1, Q2, Q3, Q4, Q5, </t>
+  </si>
+  <si>
+    <t>Q_NMOS_DGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1, </t>
+  </si>
+  <si>
+    <t>10ohm</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>10 ohm (₹12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2, R3, </t>
+  </si>
+  <si>
+    <t>5k</t>
+  </si>
+  <si>
+    <t>5k ohm (₹1.28/10 piece)</t>
+  </si>
+  <si>
+    <t>5.1k ohm (₹1.99/10 piece)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4, R21, </t>
+  </si>
+  <si>
+    <t>220 ohm</t>
+  </si>
+  <si>
+    <t>220 ohm_0402 (₹1.67/20 piece)</t>
+  </si>
+  <si>
+    <t>220 ohm (₹45.87/10 piece)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5, R6, R8, R9, R10, R11, R13, R14, R15, R22, </t>
+  </si>
+  <si>
+    <t>4.7k ohm (₹0.39/100 piece)</t>
+  </si>
+  <si>
+    <t>4.7k ohm (₹2.56/10 piece)</t>
+  </si>
+  <si>
+    <t>4.7k ohm (₹0.72/10 piece)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7, R12, R23, R24, </t>
+  </si>
+  <si>
+    <t>100 ohm</t>
+  </si>
+  <si>
+    <t>100 ohm_0603 (₹0.45/100 piece)</t>
+  </si>
+  <si>
+    <t>100 ohm (₹1.2/10 piece)</t>
+  </si>
+  <si>
+    <t>100 ohm (₹24.88/10 piece)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R16, R17, R18, R19, R20, </t>
+  </si>
+  <si>
+    <t>10k ohm(₹0.6/20 piece)</t>
+  </si>
+  <si>
+    <t>10k ohm (₹1.2/10 piece)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R25, </t>
+  </si>
+  <si>
+    <t>47k</t>
+  </si>
+  <si>
+    <t>47k ohm (₹0.6/20 piece)</t>
+  </si>
+  <si>
+    <t>47k ohm (₹0.96/10 piece)</t>
+  </si>
+  <si>
+    <t>47k ohm (₹34.74/10 piece)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1, SW2, </t>
+  </si>
+  <si>
+    <t>Button_Switch_SMD:SW_SPST_CK_RS282G05A3</t>
+  </si>
+  <si>
+    <t>sw_push H6.0mm (165.36)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2, </t>
+  </si>
+  <si>
+    <t>TLV1117LV30DCYT</t>
+  </si>
+  <si>
+    <t>AMS1117-3.3</t>
+  </si>
+  <si>
+    <t>SOT230P700X180-4N:SOT230P700X180-4N</t>
+  </si>
+  <si>
+    <t>1A Low Dropout regulator, positive, 3.3V fixed output, SOT-223</t>
+  </si>
+  <si>
+    <t>AMS-1117-3.3 (₹13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3, </t>
+  </si>
+  <si>
     <t>DRV8833PW</t>
   </si>
   <si>
     <t>Package_SO:TSSOP-16_4.4x5mm_P0.65mm</t>
-  </si>
-  <si>
-    <t>Dual H-Bridge Motor Driver, TSSOP-16</t>
-  </si>
-  <si>
-    <t>C50506</t>
-  </si>
-  <si>
-    <t>U4,</t>
-  </si>
-  <si>
-    <t>VL6180XV0NR/1</t>
-  </si>
-  <si>
-    <t>VL6180XV0NR_1:LGA12R75P2X6_280X480X110</t>
-  </si>
-  <si>
-    <t>ToF</t>
-  </si>
-  <si>
-    <t>tanotis</t>
-  </si>
-  <si>
-    <t>C2688732</t>
-  </si>
-  <si>
-    <t>U5,</t>
-  </si>
-  <si>
-    <t>MPU-6500</t>
-  </si>
-  <si>
-    <t>MPU-6500:QFN40P300X300X95-25N</t>
-  </si>
-  <si>
-    <t>IMU</t>
-  </si>
-  <si>
-    <t>Not available in India (from module)</t>
-  </si>
-  <si>
-    <t>C50278</t>
-  </si>
-  <si>
-    <t>U6,</t>
-  </si>
-  <si>
-    <t>STM32F405RGT6</t>
-  </si>
-  <si>
-    <t>Package_QFP:LQFP-64_10x10mm_P0.5mm</t>
-  </si>
-  <si>
-    <t>ARM Cortex-M4 MCU, 1024KB flash, 128KB RAM, 168MHz, 1.8-3.6V, 51 GPIO, LQFP-64</t>
-  </si>
-  <si>
-    <t>C15742</t>
-  </si>
-  <si>
-    <t>Y1,</t>
-  </si>
-  <si>
-    <t>25Mhz</t>
-  </si>
-  <si>
-    <t>EC-9631</t>
-  </si>
-  <si>
-    <t>Crystal:Crystal_SMD_3225-4Pin_3.2x2.5mm</t>
-  </si>
-  <si>
-    <t>Four pin crystal, GND on pins 2 and 4</t>
-  </si>
-  <si>
-    <t>electronicscomp</t>
-  </si>
-  <si>
-    <t>C295525</t>
-  </si>
-  <si>
-    <t>Y2,</t>
-  </si>
-  <si>
-    <t>32.768kHz</t>
-  </si>
-  <si>
-    <t>X3215-32.768K-12.5</t>
-  </si>
-  <si>
-    <t>ABS07-32:XTAL_ABS07-32.768KHZ-T</t>
-  </si>
-  <si>
-    <t>Two pin crystal</t>
-  </si>
-  <si>
-    <t>assign footprint</t>
-  </si>
-  <si>
-    <t>C93228</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of SMD components = </t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>di</t>
-  </si>
-  <si>
-    <t>Comp name</t>
-  </si>
-  <si>
-    <t>Best Buy (₹) /peice</t>
-  </si>
-  <si>
-    <t>Overall cost (₹)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A1, A2, A3, A4, </t>
-  </si>
-  <si>
-    <t>Photo-Transistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not available on Indian sites </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BZ1, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1, C2, C27, </t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>C417153_$0.09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3, C4, C30, C32, C33, </t>
-  </si>
-  <si>
-    <t>pack of 50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C8, C13, </t>
-  </si>
-  <si>
-    <t>47uF</t>
-  </si>
-  <si>
-    <t>47uf_0603 (₹30.84/10 piece)</t>
-  </si>
-  <si>
-    <t>47uF_0603 (₹36.97/10 piece)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C11, C15, </t>
-  </si>
-  <si>
-    <t>20pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C12, C19, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C20, C21, </t>
-  </si>
-  <si>
-    <t>12.5pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C22, C24, C28, C18, </t>
-  </si>
-  <si>
-    <t>10uF_0402 (₹10.07/10 piece)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C7, C9, C10, C14, C16, , C23, C25, </t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>100nF_0402 (₹1.78/40 piece)</t>
-  </si>
-  <si>
-    <t>too costly</t>
-  </si>
-  <si>
-    <t>100nF_0402 (₹2.86/10 piece)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C26, C17, </t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>10nF_0603 (₹2/50 piece)</t>
-  </si>
-  <si>
-    <t>10nF_0402 (₹8.79/10 piece)</t>
-  </si>
-  <si>
-    <t>10nF_0402 (₹13.28/10 piece)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C29, </t>
-  </si>
-  <si>
-    <t>4.7uF_0603 (₹1.8/10 piece)</t>
-  </si>
-  <si>
-    <t>4.7_0402 (₹21.97/10 piece)</t>
-  </si>
-  <si>
-    <t>4.7uF_0402 (₹19.16/10 piece)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C31, </t>
-  </si>
-  <si>
-    <t>0.01uF_0603 (₹1.8/10 piece)</t>
-  </si>
-  <si>
-    <t>(0.01uF (₹10.31/10 piece)</t>
-  </si>
-  <si>
-    <t>0.01uF (₹11.93/10 piece)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1, D6, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">D2, D3, D4, D5, </t>
-  </si>
-  <si>
-    <t>IR LED Transmitter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB1, </t>
-  </si>
-  <si>
-    <t>FerriteBead_Small</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC1, IC2, </t>
-  </si>
-  <si>
-    <t>AS5600-ASOT</t>
-  </si>
-  <si>
-    <t>AS5600-ASOT:SOIC127P600X175-8N</t>
-  </si>
-  <si>
-    <t>AS5600-ASOT (₹269.26)</t>
-  </si>
-  <si>
-    <t>AS5600-ASOT (₹267.92)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1, </t>
-  </si>
-  <si>
-    <t>Connector_JST:JST_SH_SM04B-SRSS-TB_1x04-1MP_P1.00mm_Horizontal</t>
-  </si>
-  <si>
-    <t>Serial Wire connector</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J2, </t>
-  </si>
-  <si>
-    <t>Power connector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q1, Q2, Q3, Q4, Q5, </t>
-  </si>
-  <si>
-    <t>Q_NMOS_DGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1, </t>
-  </si>
-  <si>
-    <t>10ohm</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>10 ohm (₹12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2, R3, </t>
-  </si>
-  <si>
-    <t>5k</t>
-  </si>
-  <si>
-    <t>5k ohm (₹1.28/10 piece)</t>
-  </si>
-  <si>
-    <t>5.1k ohm (₹1.99/10 piece)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4, R21, </t>
-  </si>
-  <si>
-    <t>220 ohm</t>
-  </si>
-  <si>
-    <t>220 ohm_0402 (₹1.67/20 piece)</t>
-  </si>
-  <si>
-    <t>220 ohm (₹45.87/10 piece)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5, R6, R8, R9, R10, R11, R13, R14, R15, R22, </t>
-  </si>
-  <si>
-    <t>4.7k ohm (₹0.39/100 piece)</t>
-  </si>
-  <si>
-    <t>4.7k ohm (₹2.56/10 piece)</t>
-  </si>
-  <si>
-    <t>4.7k ohm (₹0.72/10 piece)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7, R12, R23, R24, </t>
-  </si>
-  <si>
-    <t>100 ohm</t>
-  </si>
-  <si>
-    <t>100 ohm_0603 (₹0.45/100 piece)</t>
-  </si>
-  <si>
-    <t>100 ohm (₹1.2/10 piece)</t>
-  </si>
-  <si>
-    <t>100 ohm (₹24.88/10 piece)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R16, R17, R18, R19, R20, </t>
-  </si>
-  <si>
-    <t>10k ohm(₹0.6/20 piece)</t>
-  </si>
-  <si>
-    <t>10k ohm (₹1.2/10 piece)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R25, </t>
-  </si>
-  <si>
-    <t>47k</t>
-  </si>
-  <si>
-    <t>47k ohm (₹0.6/20 piece)</t>
-  </si>
-  <si>
-    <t>47k ohm (₹0.96/10 piece)</t>
-  </si>
-  <si>
-    <t>47k ohm (₹34.74/10 piece)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW1, SW2, </t>
-  </si>
-  <si>
-    <t>Button_Switch_SMD:SW_SPST_CK_RS282G05A3</t>
-  </si>
-  <si>
-    <t>sw_push H6.0mm (165.36)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2, </t>
-  </si>
-  <si>
-    <t>TLV1117LV30DCYT</t>
-  </si>
-  <si>
-    <t>AMS1117-3.3</t>
-  </si>
-  <si>
-    <t>SOT230P700X180-4N:SOT230P700X180-4N</t>
-  </si>
-  <si>
-    <t>1A Low Dropout regulator, positive, 3.3V fixed output, SOT-223</t>
-  </si>
-  <si>
-    <t>AMS-1117-3.3 (₹13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U3, </t>
   </si>
   <si>
     <t>DRV8833 (₹99)</t>
@@ -1985,13 +1991,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="51.0"/>
+    <col customWidth="1" min="1" max="1" width="65.75"/>
     <col customWidth="1" min="2" max="2" width="8.0"/>
     <col customWidth="1" min="3" max="3" width="17.63"/>
     <col customWidth="1" min="4" max="5" width="28.75"/>
@@ -3803,7 +3810,7 @@
       <c r="D32" s="84" t="s">
         <v>169</v>
       </c>
-      <c r="E32" s="83" t="s">
+      <c r="E32" s="84" t="s">
         <v>170</v>
       </c>
       <c r="F32" s="83" t="s">
@@ -4390,6 +4397,9 @@
     <hyperlink r:id="rId68" ref="I37"/>
     <hyperlink r:id="rId69" ref="P37"/>
   </hyperlinks>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToWidth="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId70"/>
 </worksheet>
 </file>
@@ -5820,19 +5830,19 @@
         <v>1.0</v>
       </c>
       <c r="C36" s="115" t="s">
-        <v>169</v>
+        <v>305</v>
       </c>
       <c r="D36" s="115" t="s">
-        <v>169</v>
+        <v>305</v>
       </c>
       <c r="E36" s="115" t="s">
-        <v>170</v>
+        <v>306</v>
       </c>
       <c r="F36" s="115" t="s">
         <v>171</v>
       </c>
       <c r="G36" s="121" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="H36" s="118" t="s">
         <v>32</v>
@@ -5856,7 +5866,7 @@
     </row>
     <row r="37">
       <c r="A37" s="115" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B37" s="115">
         <v>1.0</v>
@@ -5865,22 +5875,22 @@
         <v>174</v>
       </c>
       <c r="D37" s="115" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E37" s="115" t="s">
         <v>175</v>
       </c>
       <c r="F37" s="115" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="G37" s="130" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="H37" s="121" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="I37" s="117" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="J37" s="123"/>
       <c r="K37" s="119">
@@ -5898,7 +5908,7 @@
     </row>
     <row r="38">
       <c r="A38" s="115" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B38" s="115">
         <v>1.0</v>
@@ -5913,13 +5923,13 @@
         <v>181</v>
       </c>
       <c r="F38" s="115" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="G38" s="121" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="H38" s="117" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="I38" s="118" t="s">
         <v>32</v>
@@ -5940,16 +5950,16 @@
     </row>
     <row r="39">
       <c r="A39" s="115" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B39" s="115">
         <v>1.0</v>
       </c>
       <c r="C39" s="115" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D39" s="115" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E39" s="115" t="s">
         <v>187</v>
@@ -5962,7 +5972,7 @@
         <v>32</v>
       </c>
       <c r="I39" s="117" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="J39" s="123"/>
       <c r="K39" s="123"/>
@@ -5978,7 +5988,7 @@
     </row>
     <row r="40">
       <c r="A40" s="115" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B40" s="115">
         <v>1.0</v>
@@ -5987,7 +5997,7 @@
         <v>191</v>
       </c>
       <c r="D40" s="115" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E40" s="115" t="s">
         <v>193</v>
@@ -5996,13 +6006,13 @@
         <v>194</v>
       </c>
       <c r="G40" s="121" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="H40" s="117" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="I40" s="117" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="J40" s="123"/>
       <c r="K40" s="119">
@@ -6020,16 +6030,16 @@
     </row>
     <row r="41">
       <c r="A41" s="115" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B41" s="115">
         <v>1.0</v>
       </c>
       <c r="C41" s="115" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D41" s="115" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E41" s="115" t="s">
         <v>200</v>
@@ -6038,13 +6048,13 @@
         <v>201</v>
       </c>
       <c r="G41" s="121" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="H41" s="117" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="I41" s="117" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="J41" s="123"/>
       <c r="K41" s="119">

</xml_diff>